<commit_message>
Updated results to include lengths of 300mm and 500mm
</commit_message>
<xml_diff>
--- a/BPA_Static_Characterization_Test/20mm_ForceLengthPressure/Pulse test results.xlsx
+++ b/BPA_Static_Characterization_Test/20mm_ForceLengthPressure/Pulse test results.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ME masters project\github\Muscle_Sensory\BPA_Static_Characterization_Test\20mm_ForceLengthPressure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0A3B466-2199-4E94-8920-1D4110C2C4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A1D2F5-3D63-403A-92D0-0C94A3D61171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7781AE6A-A05B-4E08-9903-F8A9B7CCFEB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{7781AE6A-A05B-4E08-9903-F8A9B7CCFEB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="369mm" sheetId="3" r:id="rId3"/>
+    <sheet name="300mm" sheetId="4" r:id="rId4"/>
+    <sheet name="509mm" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
   <si>
     <t>Pulse duration (ms)</t>
   </si>
@@ -147,6 +149,30 @@
   <si>
     <t>j41</t>
   </si>
+  <si>
+    <t>length (cm)</t>
+  </si>
+  <si>
+    <t>day 1</t>
+  </si>
+  <si>
+    <t>day 2</t>
+  </si>
+  <si>
+    <t>dial reading (kPa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital pressure reading </t>
+  </si>
+  <si>
+    <t>j61</t>
+  </si>
+  <si>
+    <t>from 297</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
 </sst>
 </file>
 
@@ -161,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,11 +224,67 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -211,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,6 +303,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,6 +892,518 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>digital pressure readings day 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40558967629046372"/>
+                  <c:y val="9.2175925925925925E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$4:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>947</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$4:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8637-4B19-B096-236FD25B35A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="364649288"/>
+        <c:axId val="364649648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="364649288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Digital Pressure readings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364649648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="364649648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dial pressure readings (kPa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364649288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
             <c:v>pressure vs strain</c:v>
           </c:tx>
           <c:spPr>
@@ -1280,6 +1882,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2312,20 +2954,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2345,6 +3503,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D7BB869-E24B-91BC-5109-BACAFE46B9B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2919,19 +4113,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A98E28B-6B90-4D08-A0E5-BC3784CAF441}">
-  <dimension ref="A3:C15"/>
+  <dimension ref="A2:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2941,8 +4145,17 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2952,71 +4165,125 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>200</v>
       </c>
       <c r="B5">
         <v>259</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>300</v>
       </c>
       <c r="B6">
         <v>399</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>180</v>
+      </c>
+      <c r="H6">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>400</v>
       </c>
       <c r="B7">
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>300</v>
+      </c>
+      <c r="H7">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>500</v>
       </c>
       <c r="B8">
         <v>683</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>405</v>
+      </c>
+      <c r="H8">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>600</v>
       </c>
       <c r="B9">
         <v>814</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>500</v>
+      </c>
+      <c r="H9">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>620</v>
       </c>
       <c r="B10">
         <v>836</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>605</v>
+      </c>
+      <c r="H10">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>700</v>
       </c>
       <c r="B11">
         <v>946</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>700</v>
+      </c>
+      <c r="H11">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>363</v>
+      </c>
+      <c r="G15">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3029,8 +4296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2708FD-2F43-4DD2-A436-851B1200C17D}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3520,7 +4787,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -4167,4 +5434,1411 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A16763-ED46-4079-BBBB-F27EBF19559A}">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1">
+        <v>297</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>225</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>(B1-B2)/B1</f>
+        <v>0.24242424242424243</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
+        <v>299</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>272</v>
+      </c>
+      <c r="B7" s="7">
+        <f>($B$1-A7)/$B$1</f>
+        <v>8.4175084175084181E-2</v>
+      </c>
+      <c r="C7" s="7">
+        <f>B7/$B$3</f>
+        <v>0.34722222222222221</v>
+      </c>
+      <c r="D7" s="7">
+        <v>206</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>252</v>
+      </c>
+      <c r="B8" s="7">
+        <f t="shared" ref="B8:B12" si="0">($B$1-A8)/$B$1</f>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" ref="C8:C12" si="1">B8/$B$3</f>
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="7">
+        <v>301</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>240</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.19191919191919191</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D9" s="7">
+        <v>399</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>233</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.21548821548821548</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D10" s="7">
+        <v>501</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>226</v>
+      </c>
+      <c r="B11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23905723905723905</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.98611111111111105</v>
+      </c>
+      <c r="D11" s="7">
+        <v>605</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>225</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.24242424242424243</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>623</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>297</v>
+      </c>
+      <c r="B14" s="8">
+        <f>($B$1-A14)/$B$1</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <f>B14/$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>625</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1122</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>297</v>
+      </c>
+      <c r="B15" s="8">
+        <f>($B$1-A15)/$B$1</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <f>B15/$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>389</v>
+      </c>
+      <c r="E15" s="8">
+        <v>743</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>298</v>
+      </c>
+      <c r="B16" s="8">
+        <f>($B$1-A16)/$B$1</f>
+        <v>-3.3670033670033669E-3</v>
+      </c>
+      <c r="C16" s="8">
+        <f>B16/$B$3</f>
+        <v>-1.3888888888888888E-2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>92</v>
+      </c>
+      <c r="E16" s="8">
+        <v>123</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>295</v>
+      </c>
+      <c r="B17" s="8">
+        <f>($B$1-A17)/$B$1</f>
+        <v>6.7340067340067337E-3</v>
+      </c>
+      <c r="C17" s="8">
+        <f>B17/$B$3</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>190</v>
+      </c>
+      <c r="E17" s="8">
+        <v>325</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>295</v>
+      </c>
+      <c r="B18" s="8">
+        <f>($B$1-A18)/$B$1</f>
+        <v>6.7340067340067337E-3</v>
+      </c>
+      <c r="C18" s="8">
+        <f>B18/$B$3</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D18" s="8">
+        <v>401</v>
+      </c>
+      <c r="E18" s="8">
+        <v>771</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>293</v>
+      </c>
+      <c r="B19" s="8">
+        <f>($B$1-A19)/$B$1</f>
+        <v>1.3468013468013467E-2</v>
+      </c>
+      <c r="C19" s="8">
+        <f>B19/$B$3</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>510</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1001</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>295</v>
+      </c>
+      <c r="B20" s="8">
+        <f>($B$1-A20)/$B$1</f>
+        <v>6.7340067340067337E-3</v>
+      </c>
+      <c r="C20" s="8">
+        <f>B20/$B$3</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D20" s="8">
+        <v>305</v>
+      </c>
+      <c r="E20" s="8">
+        <v>564</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>297</v>
+      </c>
+      <c r="B21" s="8">
+        <f>($B$1-A21)/$B$1</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <f>B21/$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>98</v>
+      </c>
+      <c r="E21" s="8">
+        <v>126</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>281</v>
+      </c>
+      <c r="B24" s="10">
+        <f>($B$1-A24)/$B$1</f>
+        <v>5.387205387205387E-2</v>
+      </c>
+      <c r="C24" s="10">
+        <f>B24/$B$3</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D24" s="10">
+        <v>175</v>
+      </c>
+      <c r="E24" s="10">
+        <v>50</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>280</v>
+      </c>
+      <c r="B25" s="10">
+        <f t="shared" ref="B25:B30" si="2">($B$1-A25)/$B$1</f>
+        <v>5.7239057239057242E-2</v>
+      </c>
+      <c r="C25" s="10">
+        <f t="shared" ref="C25:C30" si="3">B25/$B$3</f>
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="D25" s="10">
+        <v>196</v>
+      </c>
+      <c r="E25" s="10">
+        <v>92</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>280</v>
+      </c>
+      <c r="B26" s="10">
+        <f t="shared" si="2"/>
+        <v>5.7239057239057242E-2</v>
+      </c>
+      <c r="C26" s="10">
+        <f t="shared" si="3"/>
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="D26" s="10">
+        <v>402</v>
+      </c>
+      <c r="E26" s="10">
+        <v>480</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>281</v>
+      </c>
+      <c r="B27" s="10">
+        <f t="shared" si="2"/>
+        <v>5.387205387205387E-2</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D27" s="10">
+        <v>409</v>
+      </c>
+      <c r="E27" s="10">
+        <v>497</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>279</v>
+      </c>
+      <c r="B28" s="10">
+        <f t="shared" si="2"/>
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="D28" s="10">
+        <v>613</v>
+      </c>
+      <c r="E28" s="10">
+        <v>865</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>278</v>
+      </c>
+      <c r="B29" s="10">
+        <f t="shared" si="2"/>
+        <v>6.3973063973063973E-2</v>
+      </c>
+      <c r="C29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="D29" s="10">
+        <v>605</v>
+      </c>
+      <c r="E29" s="10">
+        <v>851</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
+        <v>280</v>
+      </c>
+      <c r="B30" s="10">
+        <f t="shared" si="2"/>
+        <v>5.7239057239057242E-2</v>
+      </c>
+      <c r="C30" s="10">
+        <f t="shared" si="3"/>
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="D30" s="10">
+        <v>285</v>
+      </c>
+      <c r="E30" s="10">
+        <v>273</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
+        <v>277</v>
+      </c>
+      <c r="B31" s="10">
+        <f>($B$1-A31)/$B$1</f>
+        <v>6.7340067340067339E-2</v>
+      </c>
+      <c r="C31" s="10">
+        <f>B31/$B$3</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D31" s="10">
+        <v>505</v>
+      </c>
+      <c r="E31" s="10">
+        <v>676</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
+        <v>282</v>
+      </c>
+      <c r="B32" s="10">
+        <f>($B$1-A32)/$B$1</f>
+        <v>5.0505050505050504E-2</v>
+      </c>
+      <c r="C32" s="10">
+        <f>B32/$B$3</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="D32" s="10">
+        <v>91</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="11">
+        <v>254</v>
+      </c>
+      <c r="B34" s="11">
+        <f>($B$1-A34)/$B$1</f>
+        <v>0.14478114478114479</v>
+      </c>
+      <c r="C34" s="11">
+        <f>B34/$B$3</f>
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D34" s="11">
+        <v>277</v>
+      </c>
+      <c r="E34" s="11">
+        <v>30</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="11">
+        <v>253</v>
+      </c>
+      <c r="B35" s="11">
+        <f>($B$1-A35)/$B$1</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="C35" s="11">
+        <f>B35/$B$3</f>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D35" s="11">
+        <v>400</v>
+      </c>
+      <c r="E35" s="11">
+        <v>177</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
+        <v>253</v>
+      </c>
+      <c r="B36" s="11">
+        <f>($B$1-A36)/$B$1</f>
+        <v>0.14814814814814814</v>
+      </c>
+      <c r="C36" s="11">
+        <f>B36/$B$3</f>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D36" s="11">
+        <v>290</v>
+      </c>
+      <c r="E36" s="11">
+        <v>49</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
+        <v>252</v>
+      </c>
+      <c r="B37" s="11">
+        <f>($B$1-A37)/$B$1</f>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="C37" s="11">
+        <f>B37/$B$3</f>
+        <v>0.625</v>
+      </c>
+      <c r="D37" s="11">
+        <v>611</v>
+      </c>
+      <c r="E37" s="11">
+        <v>423</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="11">
+        <v>252</v>
+      </c>
+      <c r="B38" s="11">
+        <f>($B$1-A38)/$B$1</f>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="C38" s="11">
+        <f>B38/$B$3</f>
+        <v>0.625</v>
+      </c>
+      <c r="D38" s="11">
+        <v>492</v>
+      </c>
+      <c r="E38" s="11">
+        <v>292</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
+        <v>254</v>
+      </c>
+      <c r="B39" s="11">
+        <f>($B$1-A39)/$B$1</f>
+        <v>0.14478114478114479</v>
+      </c>
+      <c r="C39" s="11">
+        <f>B39/$B$3</f>
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D39" s="11">
+        <v>353</v>
+      </c>
+      <c r="E39" s="11">
+        <v>135</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="11">
+        <v>252</v>
+      </c>
+      <c r="B40" s="11">
+        <f>($B$1-A40)/$B$1</f>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="C40" s="11">
+        <f>B40/$B$3</f>
+        <v>0.625</v>
+      </c>
+      <c r="D40" s="11">
+        <v>598</v>
+      </c>
+      <c r="E40" s="11">
+        <v>416</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="12">
+        <v>241</v>
+      </c>
+      <c r="B42" s="12">
+        <f>($B$1-A42)/$B$1</f>
+        <v>0.18855218855218855</v>
+      </c>
+      <c r="C42" s="12">
+        <f>B42/$B$3</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D42" s="12">
+        <v>609</v>
+      </c>
+      <c r="E42" s="12">
+        <v>258</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>241</v>
+      </c>
+      <c r="B43" s="12">
+        <f>($B$1-A43)/$B$1</f>
+        <v>0.18855218855218855</v>
+      </c>
+      <c r="C43" s="12">
+        <f>B43/$B$3</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D43" s="12">
+        <v>626</v>
+      </c>
+      <c r="E43" s="12">
+        <v>279</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="12">
+        <v>241</v>
+      </c>
+      <c r="B44" s="12">
+        <f>($B$1-A44)/$B$1</f>
+        <v>0.18855218855218855</v>
+      </c>
+      <c r="C44" s="12">
+        <f>B44/$B$3</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D44" s="12">
+        <v>494</v>
+      </c>
+      <c r="E44" s="12">
+        <v>166</v>
+      </c>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="12">
+        <v>242</v>
+      </c>
+      <c r="B45" s="12">
+        <f>($B$1-A45)/$B$1</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="C45" s="12">
+        <f>B45/$B$3</f>
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D45" s="12">
+        <v>298</v>
+      </c>
+      <c r="E45" s="12">
+        <v>2.25</v>
+      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="12">
+        <v>242</v>
+      </c>
+      <c r="B46" s="12">
+        <f>($B$1-A46)/$B$1</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="C46" s="12">
+        <f>B46/$B$3</f>
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D46" s="12">
+        <v>400</v>
+      </c>
+      <c r="E46" s="12">
+        <v>86</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="12">
+        <v>240</v>
+      </c>
+      <c r="B47" s="12">
+        <f>($B$1-A47)/$B$1</f>
+        <v>0.19191919191919191</v>
+      </c>
+      <c r="C47" s="12">
+        <f>B47/$B$3</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D47" s="12">
+        <v>350</v>
+      </c>
+      <c r="E47" s="12">
+        <v>44</v>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="12">
+        <v>242</v>
+      </c>
+      <c r="B48" s="12">
+        <f>($B$1-A48)/$B$1</f>
+        <v>0.18518518518518517</v>
+      </c>
+      <c r="C48" s="12">
+        <f>B48/$B$3</f>
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D48" s="12">
+        <v>330</v>
+      </c>
+      <c r="E48" s="12">
+        <v>25</v>
+      </c>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBF1152-E7B1-408E-98FD-CDD3D8B4640C}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1">
+        <v>509</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>385</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>(B1-B2)/B1</f>
+        <v>0.24361493123772102</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>385</v>
+      </c>
+      <c r="B6" s="13">
+        <f>($B$1-A6)/$B$1</f>
+        <v>0.24361493123772102</v>
+      </c>
+      <c r="C6" s="13">
+        <f>B6/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>620</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>391</v>
+      </c>
+      <c r="B7" s="13">
+        <f t="shared" ref="B7:B11" si="0">($B$1-A7)/$B$1</f>
+        <v>0.23182711198428291</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" ref="C7:C11" si="1">B7/$B$3</f>
+        <v>0.95161290322580649</v>
+      </c>
+      <c r="D7" s="14">
+        <v>500</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>400</v>
+      </c>
+      <c r="B8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.21414538310412573</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="1"/>
+        <v>0.87903225806451613</v>
+      </c>
+      <c r="D8" s="14">
+        <v>394</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>413</v>
+      </c>
+      <c r="B9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.18860510805500982</v>
+      </c>
+      <c r="C9" s="13">
+        <f t="shared" si="1"/>
+        <v>0.77419354838709675</v>
+      </c>
+      <c r="D9" s="14">
+        <v>295</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>445</v>
+      </c>
+      <c r="B10" s="13">
+        <f t="shared" si="0"/>
+        <v>0.12573673870333987</v>
+      </c>
+      <c r="C10" s="13">
+        <f t="shared" si="1"/>
+        <v>0.5161290322580645</v>
+      </c>
+      <c r="D10" s="14">
+        <v>191</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>488</v>
+      </c>
+      <c r="B11" s="13">
+        <f t="shared" si="0"/>
+        <v>4.1257367387033402E-2</v>
+      </c>
+      <c r="C11" s="13">
+        <f t="shared" si="1"/>
+        <v>0.16935483870967744</v>
+      </c>
+      <c r="D11" s="14">
+        <v>95</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>485</v>
+      </c>
+      <c r="B13" s="11">
+        <f>($B$1-A13)/$B$1</f>
+        <v>4.7151277013752456E-2</v>
+      </c>
+      <c r="C13" s="11">
+        <f>B13/$B$3</f>
+        <v>0.19354838709677419</v>
+      </c>
+      <c r="D13" s="11">
+        <v>615</v>
+      </c>
+      <c r="E13" s="11">
+        <v>1057</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11">
+        <f t="shared" ref="B14:B19" si="2">($B$1-A14)/$B$1</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" ref="C14:C19" si="3">B14/$B$3</f>
+        <v>4.104838709677419</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="3"/>
+        <v>4.104838709677419</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.104838709677419</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="3"/>
+        <v>4.104838709677419</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="3"/>
+        <v>4.104838709677419</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" si="3"/>
+        <v>4.104838709677419</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>